<commit_message>
ok les formules je confirme
</commit_message>
<xml_diff>
--- a/resultatsEvscape.xlsx
+++ b/resultatsEvscape.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="36">
   <si>
     <t>Boudlal</t>
   </si>
@@ -23,28 +23,76 @@
     <t>Khalid</t>
   </si>
   <si>
+    <t>abstention</t>
+  </si>
+  <si>
     <t>reponseC</t>
   </si>
   <si>
+    <t>reponseB</t>
+  </si>
+  <si>
+    <t>Reponse1Spec1</t>
+  </si>
+  <si>
+    <t>responseA</t>
+  </si>
+  <si>
+    <t>Reponse7Spec1</t>
+  </si>
+  <si>
+    <t>Reponse8Spec1</t>
+  </si>
+  <si>
+    <t>Reponse9Spec1</t>
+  </si>
+  <si>
+    <t>Reponse10Spec1</t>
+  </si>
+  <si>
+    <t>Gisele</t>
+  </si>
+  <si>
+    <t>Giligi</t>
+  </si>
+  <si>
+    <t>Reponse3Spec1</t>
+  </si>
+  <si>
+    <t>Reponse4Spec1</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>lie</t>
+  </si>
+  <si>
+    <t>Reponse5Spec1</t>
+  </si>
+  <si>
     <t>Reponse2Spec1</t>
   </si>
   <si>
-    <t>responseA</t>
-  </si>
-  <si>
-    <t>reponseB</t>
-  </si>
-  <si>
-    <t>Reponse7Spec1</t>
-  </si>
-  <si>
-    <t>Reponse10Spec1</t>
-  </si>
-  <si>
-    <t>Reponse1Spec1</t>
-  </si>
-  <si>
-    <t>Reponse3Spec1</t>
+    <t>Gele</t>
+  </si>
+  <si>
+    <t>Gigi</t>
+  </si>
+  <si>
+    <t>Reponse6Spec1</t>
+  </si>
+  <si>
+    <t>Patrke</t>
+  </si>
+  <si>
+    <t>Klert</t>
+  </si>
+  <si>
+    <t>Berrd</t>
+  </si>
+  <si>
+    <t>Aert</t>
   </si>
   <si>
     <t>Tozer</t>
@@ -53,36 +101,18 @@
     <t>Elie</t>
   </si>
   <si>
-    <t>Reponse6Spec1</t>
-  </si>
-  <si>
-    <t>Reponse8Spec1</t>
-  </si>
-  <si>
     <t>Lita</t>
   </si>
   <si>
     <t>Zoe</t>
   </si>
   <si>
-    <t>Reponse4Spec1</t>
-  </si>
-  <si>
-    <t>Reponse9Spec1</t>
-  </si>
-  <si>
     <t>toto</t>
   </si>
   <si>
     <t>litoe</t>
   </si>
   <si>
-    <t>Gisele</t>
-  </si>
-  <si>
-    <t>Giligi</t>
-  </si>
-  <si>
     <t>Patricke</t>
   </si>
   <si>
@@ -93,33 +123,6 @@
   </si>
   <si>
     <t>Albert</t>
-  </si>
-  <si>
-    <t>Reponse5Spec1</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>lie</t>
-  </si>
-  <si>
-    <t>Gele</t>
-  </si>
-  <si>
-    <t>Gigi</t>
-  </si>
-  <si>
-    <t>Patrke</t>
-  </si>
-  <si>
-    <t>Klert</t>
-  </si>
-  <si>
-    <t>Berrd</t>
-  </si>
-  <si>
-    <t>Aert</t>
   </si>
 </sst>
 </file>
@@ -459,13 +462,13 @@
   <sheetData>
     <row r="30" spans="1:24">
       <c r="A30">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D30" t="b">
         <v>0</v>
@@ -474,146 +477,146 @@
         <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G30" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H30" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I30" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="J30" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K30" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L30" t="s">
+        <v>2</v>
+      </c>
+      <c r="M30" t="s">
+        <v>3</v>
+      </c>
+      <c r="N30" t="s">
+        <v>4</v>
+      </c>
+      <c r="O30" t="s">
+        <v>2</v>
+      </c>
+      <c r="P30" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q30" t="s">
         <v>13</v>
       </c>
-      <c r="M30" t="s">
-        <v>17</v>
-      </c>
-      <c r="N30" t="s">
+      <c r="R30" t="s">
+        <v>2</v>
+      </c>
+      <c r="S30" t="s">
+        <v>3</v>
+      </c>
+      <c r="T30" t="s">
+        <v>21</v>
+      </c>
+      <c r="U30" t="s">
         <v>7</v>
       </c>
-      <c r="O30" t="s">
-        <v>8</v>
-      </c>
-      <c r="P30" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q30" t="s">
+      <c r="V30" t="s">
+        <v>2</v>
+      </c>
+      <c r="W30" t="s">
         <v>9</v>
       </c>
-      <c r="R30" t="s">
-        <v>4</v>
-      </c>
-      <c r="S30" t="s">
-        <v>26</v>
-      </c>
-      <c r="T30" t="s">
-        <v>5</v>
-      </c>
-      <c r="U30" t="s">
-        <v>6</v>
-      </c>
-      <c r="V30" t="s">
-        <v>13</v>
-      </c>
-      <c r="W30" t="s">
-        <v>17</v>
-      </c>
       <c r="X30" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:24">
       <c r="A31">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
       </c>
       <c r="E31" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G31" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H31" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="I31" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J31" t="s">
         <v>2</v>
       </c>
       <c r="K31" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L31" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M31" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N31" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="O31" t="s">
+        <v>2</v>
+      </c>
+      <c r="P31" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>13</v>
+      </c>
+      <c r="R31" t="s">
+        <v>4</v>
+      </c>
+      <c r="S31" t="s">
+        <v>2</v>
+      </c>
+      <c r="T31" t="s">
+        <v>21</v>
+      </c>
+      <c r="U31" t="s">
+        <v>2</v>
+      </c>
+      <c r="V31" t="s">
         <v>8</v>
       </c>
-      <c r="P31" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>4</v>
-      </c>
-      <c r="R31" t="s">
-        <v>16</v>
-      </c>
-      <c r="S31" t="s">
-        <v>26</v>
-      </c>
-      <c r="T31" t="s">
-        <v>2</v>
-      </c>
-      <c r="U31" t="s">
-        <v>2</v>
-      </c>
-      <c r="V31" t="s">
-        <v>13</v>
-      </c>
       <c r="W31" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="X31" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:24">
       <c r="A32">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D32" t="b">
         <v>0</v>
@@ -622,72 +625,72 @@
         <v>4</v>
       </c>
       <c r="F32" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G32" t="s">
         <v>4</v>
       </c>
       <c r="H32" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="I32" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J32" t="s">
+        <v>21</v>
+      </c>
+      <c r="K32" t="s">
+        <v>2</v>
+      </c>
+      <c r="L32" t="s">
+        <v>2</v>
+      </c>
+      <c r="M32" t="s">
+        <v>4</v>
+      </c>
+      <c r="N32" t="s">
+        <v>3</v>
+      </c>
+      <c r="O32" t="s">
         <v>5</v>
       </c>
-      <c r="K32" t="s">
-        <v>4</v>
-      </c>
-      <c r="L32" t="s">
-        <v>5</v>
-      </c>
-      <c r="M32" t="s">
-        <v>2</v>
-      </c>
-      <c r="N32" t="s">
-        <v>5</v>
-      </c>
-      <c r="O32" t="s">
-        <v>8</v>
-      </c>
       <c r="P32" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="Q32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R32" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="S32" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="T32" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="U32" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V32" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="W32" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="X32" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:24">
       <c r="A33">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
@@ -696,135 +699,135 @@
         <v>5</v>
       </c>
       <c r="F33" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G33" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H33" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="I33" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J33" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K33" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L33" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M33" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N33" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="O33" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P33" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="Q33" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="R33" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="S33" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="T33" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="U33" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="V33" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="W33" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="X33" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:24">
       <c r="A34">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C34" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D34" t="b">
         <v>0</v>
       </c>
       <c r="E34" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" t="s">
+        <v>2</v>
+      </c>
+      <c r="J34" t="s">
+        <v>4</v>
+      </c>
+      <c r="K34" t="s">
+        <v>2</v>
+      </c>
+      <c r="L34" t="s">
+        <v>2</v>
+      </c>
+      <c r="M34" t="s">
+        <v>4</v>
+      </c>
+      <c r="N34" t="s">
+        <v>2</v>
+      </c>
+      <c r="O34" t="s">
+        <v>5</v>
+      </c>
+      <c r="P34" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>13</v>
+      </c>
+      <c r="R34" t="s">
+        <v>14</v>
+      </c>
+      <c r="S34" t="s">
+        <v>17</v>
+      </c>
+      <c r="T34" t="s">
+        <v>2</v>
+      </c>
+      <c r="U34" t="s">
+        <v>2</v>
+      </c>
+      <c r="V34" t="s">
         <v>8</v>
       </c>
-      <c r="F34" t="s">
-        <v>3</v>
-      </c>
-      <c r="G34" t="s">
-        <v>2</v>
-      </c>
-      <c r="H34" t="s">
-        <v>2</v>
-      </c>
-      <c r="I34" t="s">
-        <v>5</v>
-      </c>
-      <c r="J34" t="s">
-        <v>5</v>
-      </c>
-      <c r="K34" t="s">
-        <v>4</v>
-      </c>
-      <c r="L34" t="s">
-        <v>13</v>
-      </c>
-      <c r="M34" t="s">
-        <v>5</v>
-      </c>
-      <c r="N34" t="s">
-        <v>2</v>
-      </c>
-      <c r="O34" t="s">
-        <v>2</v>
-      </c>
-      <c r="P34" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>9</v>
-      </c>
-      <c r="R34" t="s">
-        <v>5</v>
-      </c>
-      <c r="S34" t="s">
-        <v>4</v>
-      </c>
-      <c r="T34" t="s">
-        <v>2</v>
-      </c>
-      <c r="U34" t="s">
-        <v>6</v>
-      </c>
-      <c r="V34" t="s">
-        <v>13</v>
-      </c>
       <c r="W34" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="X34" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -857,280 +860,280 @@
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G24" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H24" t="s">
         <v>4</v>
       </c>
       <c r="I24" t="s">
+        <v>4</v>
+      </c>
+      <c r="J24" t="s">
+        <v>3</v>
+      </c>
+      <c r="K24" t="s">
+        <v>2</v>
+      </c>
+      <c r="L24" t="s">
+        <v>2</v>
+      </c>
+      <c r="M24" t="s">
+        <v>2</v>
+      </c>
+      <c r="N24" t="s">
+        <v>2</v>
+      </c>
+      <c r="O24" t="s">
         <v>5</v>
       </c>
-      <c r="J24" t="s">
-        <v>4</v>
-      </c>
-      <c r="K24" t="s">
-        <v>6</v>
-      </c>
-      <c r="L24" t="s">
-        <v>5</v>
-      </c>
-      <c r="M24" t="s">
-        <v>2</v>
-      </c>
-      <c r="N24" t="s">
+      <c r="P24" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>2</v>
+      </c>
+      <c r="R24" t="s">
+        <v>2</v>
+      </c>
+      <c r="S24" t="s">
+        <v>6</v>
+      </c>
+      <c r="T24" t="s">
+        <v>6</v>
+      </c>
+      <c r="U24" t="s">
         <v>7</v>
       </c>
-      <c r="O24" t="s">
+      <c r="V24" t="s">
         <v>8</v>
       </c>
-      <c r="P24" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q24" t="s">
+      <c r="W24" t="s">
         <v>9</v>
       </c>
-      <c r="R24" t="s">
-        <v>4</v>
-      </c>
-      <c r="S24" t="s">
-        <v>4</v>
-      </c>
-      <c r="T24" t="s">
-        <v>5</v>
-      </c>
-      <c r="U24" t="s">
-        <v>6</v>
-      </c>
-      <c r="V24" t="s">
-        <v>5</v>
-      </c>
-      <c r="W24" t="s">
-        <v>2</v>
-      </c>
       <c r="X24" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:24">
       <c r="A25">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D25" t="b">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G25" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="H25" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="I25" t="s">
         <v>2</v>
       </c>
       <c r="J25" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="K25" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L25" t="s">
+        <v>2</v>
+      </c>
+      <c r="M25" t="s">
+        <v>4</v>
+      </c>
+      <c r="N25" t="s">
+        <v>6</v>
+      </c>
+      <c r="O25" t="s">
+        <v>2</v>
+      </c>
+      <c r="P25" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q25" t="s">
         <v>13</v>
       </c>
-      <c r="M25" t="s">
-        <v>5</v>
-      </c>
-      <c r="N25" t="s">
-        <v>5</v>
-      </c>
-      <c r="O25" t="s">
-        <v>8</v>
-      </c>
-      <c r="P25" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q25" t="s">
-        <v>2</v>
-      </c>
       <c r="R25" t="s">
         <v>2</v>
       </c>
       <c r="S25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="T25" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="U25" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="V25" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="W25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X25" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:24">
       <c r="A26">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D26" t="b">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F26" t="s">
         <v>3</v>
       </c>
       <c r="G26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I26" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="J26" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K26" t="s">
         <v>2</v>
       </c>
       <c r="L26" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M26" t="s">
         <v>2</v>
       </c>
       <c r="N26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O26" t="s">
+        <v>2</v>
+      </c>
+      <c r="P26" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>6</v>
+      </c>
+      <c r="R26" t="s">
+        <v>3</v>
+      </c>
+      <c r="S26" t="s">
+        <v>17</v>
+      </c>
+      <c r="T26" t="s">
+        <v>2</v>
+      </c>
+      <c r="U26" t="s">
+        <v>2</v>
+      </c>
+      <c r="V26" t="s">
         <v>8</v>
       </c>
-      <c r="P26" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>2</v>
-      </c>
-      <c r="R26" t="s">
-        <v>16</v>
-      </c>
-      <c r="S26" t="s">
-        <v>2</v>
-      </c>
-      <c r="T26" t="s">
-        <v>4</v>
-      </c>
-      <c r="U26" t="s">
-        <v>6</v>
-      </c>
-      <c r="V26" t="s">
-        <v>13</v>
-      </c>
       <c r="W26" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="X26" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:24">
       <c r="A27">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D27" t="b">
         <v>1</v>
       </c>
       <c r="E27" t="s">
+        <v>4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>18</v>
+      </c>
+      <c r="G27" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" t="s">
+        <v>2</v>
+      </c>
+      <c r="J27" t="s">
+        <v>2</v>
+      </c>
+      <c r="K27" t="s">
+        <v>2</v>
+      </c>
+      <c r="L27" t="s">
+        <v>2</v>
+      </c>
+      <c r="M27" t="s">
+        <v>2</v>
+      </c>
+      <c r="N27" t="s">
+        <v>2</v>
+      </c>
+      <c r="O27" t="s">
+        <v>5</v>
+      </c>
+      <c r="P27" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>13</v>
+      </c>
+      <c r="R27" t="s">
+        <v>2</v>
+      </c>
+      <c r="S27" t="s">
+        <v>3</v>
+      </c>
+      <c r="T27" t="s">
+        <v>21</v>
+      </c>
+      <c r="U27" t="s">
+        <v>2</v>
+      </c>
+      <c r="V27" t="s">
         <v>8</v>
       </c>
-      <c r="F27" t="s">
-        <v>5</v>
-      </c>
-      <c r="G27" t="s">
+      <c r="W27" t="s">
         <v>9</v>
-      </c>
-      <c r="H27" t="s">
-        <v>16</v>
-      </c>
-      <c r="I27" t="s">
-        <v>5</v>
-      </c>
-      <c r="J27" t="s">
-        <v>5</v>
-      </c>
-      <c r="K27" t="s">
-        <v>5</v>
-      </c>
-      <c r="L27" t="s">
-        <v>13</v>
-      </c>
-      <c r="M27" t="s">
-        <v>4</v>
-      </c>
-      <c r="N27" t="s">
-        <v>4</v>
-      </c>
-      <c r="O27" t="s">
-        <v>8</v>
-      </c>
-      <c r="P27" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>9</v>
-      </c>
-      <c r="R27" t="s">
-        <v>4</v>
-      </c>
-      <c r="S27" t="s">
-        <v>4</v>
-      </c>
-      <c r="T27" t="s">
-        <v>4</v>
-      </c>
-      <c r="U27" t="s">
-        <v>6</v>
-      </c>
-      <c r="V27" t="s">
-        <v>13</v>
-      </c>
-      <c r="W27" t="s">
-        <v>17</v>
       </c>
       <c r="X27" t="s">
         <v>2</v>
@@ -1138,87 +1141,87 @@
     </row>
     <row r="28" spans="1:24">
       <c r="A28">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D28" t="b">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F28" t="s">
         <v>4</v>
       </c>
       <c r="G28" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28" t="s">
+        <v>2</v>
+      </c>
+      <c r="I28" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" t="s">
+        <v>6</v>
+      </c>
+      <c r="K28" t="s">
+        <v>6</v>
+      </c>
+      <c r="L28" t="s">
+        <v>2</v>
+      </c>
+      <c r="M28" t="s">
+        <v>4</v>
+      </c>
+      <c r="N28" t="s">
+        <v>2</v>
+      </c>
+      <c r="O28" t="s">
         <v>5</v>
       </c>
-      <c r="H28" t="s">
-        <v>5</v>
-      </c>
-      <c r="I28" t="s">
-        <v>4</v>
-      </c>
-      <c r="J28" t="s">
-        <v>4</v>
-      </c>
-      <c r="K28" t="s">
-        <v>2</v>
-      </c>
-      <c r="L28" t="s">
+      <c r="P28" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q28" t="s">
         <v>13</v>
       </c>
-      <c r="M28" t="s">
-        <v>5</v>
-      </c>
-      <c r="N28" t="s">
-        <v>2</v>
-      </c>
-      <c r="O28" t="s">
-        <v>4</v>
-      </c>
-      <c r="P28" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q28" t="s">
+      <c r="R28" t="s">
+        <v>6</v>
+      </c>
+      <c r="S28" t="s">
+        <v>4</v>
+      </c>
+      <c r="T28" t="s">
+        <v>2</v>
+      </c>
+      <c r="U28" t="s">
+        <v>7</v>
+      </c>
+      <c r="V28" t="s">
+        <v>2</v>
+      </c>
+      <c r="W28" t="s">
         <v>9</v>
       </c>
-      <c r="R28" t="s">
-        <v>2</v>
-      </c>
-      <c r="S28" t="s">
-        <v>5</v>
-      </c>
-      <c r="T28" t="s">
-        <v>2</v>
-      </c>
-      <c r="U28" t="s">
-        <v>2</v>
-      </c>
-      <c r="V28" t="s">
-        <v>13</v>
-      </c>
-      <c r="W28" t="s">
-        <v>2</v>
-      </c>
       <c r="X28" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:24">
       <c r="A29">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C29" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D29" t="b">
         <v>1</v>
@@ -1227,61 +1230,61 @@
         <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H29" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I29" t="s">
         <v>2</v>
       </c>
       <c r="J29" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="K29" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L29" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M29" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="N29" t="s">
         <v>2</v>
       </c>
       <c r="O29" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="P29" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="Q29" t="s">
+        <v>3</v>
+      </c>
+      <c r="R29" t="s">
+        <v>4</v>
+      </c>
+      <c r="S29" t="s">
+        <v>3</v>
+      </c>
+      <c r="T29" t="s">
+        <v>21</v>
+      </c>
+      <c r="U29" t="s">
+        <v>7</v>
+      </c>
+      <c r="V29" t="s">
+        <v>2</v>
+      </c>
+      <c r="W29" t="s">
         <v>9</v>
       </c>
-      <c r="R29" t="s">
-        <v>4</v>
-      </c>
-      <c r="S29" t="s">
-        <v>4</v>
-      </c>
-      <c r="T29" t="s">
-        <v>5</v>
-      </c>
-      <c r="U29" t="s">
-        <v>6</v>
-      </c>
-      <c r="V29" t="s">
-        <v>13</v>
-      </c>
-      <c r="W29" t="s">
-        <v>17</v>
-      </c>
       <c r="X29" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resultats dans specification ok
</commit_message>
<xml_diff>
--- a/resultatsEvscape.xlsx
+++ b/resultatsEvscape.xlsx
@@ -17,67 +17,94 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="36">
   <si>
+    <t>Lita</t>
+  </si>
+  <si>
+    <t>Zoe</t>
+  </si>
+  <si>
+    <t>Reponse1Spec1</t>
+  </si>
+  <si>
+    <t>abstention</t>
+  </si>
+  <si>
+    <t>reponseB</t>
+  </si>
+  <si>
+    <t>responseA</t>
+  </si>
+  <si>
+    <t>reponseC</t>
+  </si>
+  <si>
+    <t>Reponse7Spec1</t>
+  </si>
+  <si>
+    <t>toto</t>
+  </si>
+  <si>
+    <t>litoe</t>
+  </si>
+  <si>
+    <t>Reponse5Spec1</t>
+  </si>
+  <si>
+    <t>Reponse8Spec1</t>
+  </si>
+  <si>
+    <t>Reponse2Spec1</t>
+  </si>
+  <si>
+    <t>Reponse3Spec1</t>
+  </si>
+  <si>
+    <t>Reponse9Spec1</t>
+  </si>
+  <si>
+    <t>Reponse10Spec1</t>
+  </si>
+  <si>
+    <t>Gisele</t>
+  </si>
+  <si>
+    <t>Giligi</t>
+  </si>
+  <si>
+    <t>Reponse6Spec1</t>
+  </si>
+  <si>
+    <t>Patricke</t>
+  </si>
+  <si>
+    <t>Kluivert</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>lie</t>
+  </si>
+  <si>
+    <t>Reponse4Spec1</t>
+  </si>
+  <si>
+    <t>Patrke</t>
+  </si>
+  <si>
+    <t>Klert</t>
+  </si>
+  <si>
     <t>Boudlal</t>
   </si>
   <si>
     <t>Khalid</t>
   </si>
   <si>
-    <t>Reponse1Spec1</t>
-  </si>
-  <si>
-    <t>abstention</t>
-  </si>
-  <si>
-    <t>reponseB</t>
-  </si>
-  <si>
-    <t>reponseC</t>
-  </si>
-  <si>
-    <t>Reponse5Spec1</t>
-  </si>
-  <si>
-    <t>Reponse6Spec1</t>
-  </si>
-  <si>
-    <t>Reponse7Spec1</t>
-  </si>
-  <si>
-    <t>responseA</t>
-  </si>
-  <si>
-    <t>Reponse4Spec1</t>
-  </si>
-  <si>
-    <t>Reponse8Spec1</t>
-  </si>
-  <si>
-    <t>Reponse9Spec1</t>
-  </si>
-  <si>
-    <t>Lita</t>
-  </si>
-  <si>
-    <t>Zoe</t>
-  </si>
-  <si>
-    <t>Reponse2Spec1</t>
-  </si>
-  <si>
-    <t>Reponse10Spec1</t>
-  </si>
-  <si>
-    <t>toto</t>
-  </si>
-  <si>
-    <t>litoe</t>
-  </si>
-  <si>
-    <t>Patricke</t>
-  </si>
-  <si>
-    <t>Kluivert</t>
+    <t>Tozer</t>
+  </si>
+  <si>
+    <t>Elie</t>
   </si>
   <si>
     <t>Bernard</t>
@@ -86,43 +113,16 @@
     <t>Albert</t>
   </si>
   <si>
+    <t>Gele</t>
+  </si>
+  <si>
+    <t>Gigi</t>
+  </si>
+  <si>
     <t>Berrd</t>
   </si>
   <si>
     <t>Aert</t>
-  </si>
-  <si>
-    <t>Reponse3Spec1</t>
-  </si>
-  <si>
-    <t>Tozer</t>
-  </si>
-  <si>
-    <t>Elie</t>
-  </si>
-  <si>
-    <t>Gisele</t>
-  </si>
-  <si>
-    <t>Giligi</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>lie</t>
-  </si>
-  <si>
-    <t>Gele</t>
-  </si>
-  <si>
-    <t>Gigi</t>
-  </si>
-  <si>
-    <t>Patrke</t>
-  </si>
-  <si>
-    <t>Klert</t>
   </si>
 </sst>
 </file>
@@ -462,7 +462,7 @@
   <sheetData>
     <row r="8" spans="1:24">
       <c r="A8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>26</v>
@@ -477,66 +477,66 @@
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J8" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="L8" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="M8" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="N8" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="O8" t="s">
         <v>2</v>
       </c>
       <c r="P8" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>13</v>
+      </c>
+      <c r="R8" t="s">
+        <v>5</v>
+      </c>
+      <c r="S8" t="s">
+        <v>6</v>
+      </c>
+      <c r="T8" t="s">
+        <v>18</v>
+      </c>
+      <c r="U8" t="s">
+        <v>3</v>
+      </c>
+      <c r="V8" t="s">
+        <v>3</v>
+      </c>
+      <c r="W8" t="s">
+        <v>14</v>
+      </c>
+      <c r="X8" t="s">
         <v>15</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>25</v>
-      </c>
-      <c r="R8" t="s">
-        <v>9</v>
-      </c>
-      <c r="S8" t="s">
-        <v>5</v>
-      </c>
-      <c r="T8" t="s">
-        <v>3</v>
-      </c>
-      <c r="U8" t="s">
-        <v>8</v>
-      </c>
-      <c r="V8" t="s">
-        <v>11</v>
-      </c>
-      <c r="W8" t="s">
-        <v>4</v>
-      </c>
-      <c r="X8" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:24">
       <c r="A9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
         <v>28</v>
@@ -548,69 +548,69 @@
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G9" t="s">
         <v>5</v>
       </c>
       <c r="H9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J9" t="s">
         <v>3</v>
       </c>
       <c r="K9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L9" t="s">
         <v>3</v>
       </c>
       <c r="M9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O9" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="P9" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="Q9" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="R9" t="s">
         <v>3</v>
       </c>
       <c r="S9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T9" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="U9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="V9" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="W9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="X9" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:24">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>30</v>
@@ -622,43 +622,43 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
         <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="K10" t="s">
         <v>3</v>
       </c>
       <c r="L10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O10" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q10" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="R10" t="s">
         <v>3</v>
@@ -667,19 +667,19 @@
         <v>3</v>
       </c>
       <c r="T10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="U10" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="V10" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="W10" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="X10" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:24">
@@ -696,69 +696,69 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F11" t="s">
         <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H11" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I11" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="J11" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="K11" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="L11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N11" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="O11" t="s">
         <v>3</v>
       </c>
       <c r="P11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Q11" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="R11" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="S11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="T11" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="U11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V11" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="W11" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="X11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:24">
       <c r="A12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>34</v>
@@ -773,13 +773,13 @@
         <v>3</v>
       </c>
       <c r="F12" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="G12" t="s">
         <v>3</v>
       </c>
       <c r="H12" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I12" t="s">
         <v>3</v>
@@ -788,46 +788,46 @@
         <v>4</v>
       </c>
       <c r="K12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L12" t="s">
         <v>3</v>
       </c>
       <c r="M12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="O12" t="s">
         <v>2</v>
       </c>
       <c r="P12" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="Q12" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="R12" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="S12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T12" t="s">
         <v>5</v>
       </c>
       <c r="U12" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="V12" t="s">
         <v>11</v>
       </c>
       <c r="W12" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="X12" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -845,7 +845,7 @@
   <sheetData>
     <row r="2" spans="1:24">
       <c r="A2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
@@ -863,99 +863,99 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" t="s">
+        <v>3</v>
+      </c>
+      <c r="P2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" t="s">
+        <v>4</v>
+      </c>
+      <c r="S2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" t="s">
+        <v>5</v>
+      </c>
+      <c r="U2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N2" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" t="s">
-        <v>3</v>
-      </c>
-      <c r="P2" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R2" t="s">
-        <v>10</v>
-      </c>
-      <c r="S2" t="s">
-        <v>9</v>
-      </c>
-      <c r="T2" t="s">
-        <v>4</v>
-      </c>
-      <c r="U2" t="s">
-        <v>3</v>
-      </c>
       <c r="V2" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="W2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="X2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:24">
       <c r="A3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3" t="s">
         <v>3</v>
       </c>
       <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
-        <v>6</v>
-      </c>
       <c r="J3" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L3" t="s">
         <v>11</v>
       </c>
       <c r="M3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N3" t="s">
         <v>4</v>
@@ -964,63 +964,63 @@
         <v>3</v>
       </c>
       <c r="P3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Q3" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="R3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="S3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V3" t="s">
         <v>11</v>
       </c>
       <c r="W3" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="X3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:24">
       <c r="A4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="J4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K4" t="s">
         <v>3</v>
@@ -1029,40 +1029,40 @@
         <v>3</v>
       </c>
       <c r="M4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N4" t="s">
         <v>3</v>
       </c>
       <c r="O4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="P4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="R4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="T4" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="U4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="V4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="W4" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="X4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -1088,19 +1088,19 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="K5" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L5" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="M5" t="s">
         <v>3</v>
@@ -1109,39 +1109,39 @@
         <v>3</v>
       </c>
       <c r="O5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5" t="s">
+        <v>6</v>
+      </c>
+      <c r="S5" t="s">
+        <v>5</v>
+      </c>
+      <c r="T5" t="s">
+        <v>6</v>
+      </c>
+      <c r="U5" t="s">
+        <v>5</v>
+      </c>
+      <c r="V5" t="s">
+        <v>11</v>
+      </c>
+      <c r="W5" t="s">
+        <v>4</v>
+      </c>
+      <c r="X5" t="s">
         <v>15</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>4</v>
-      </c>
-      <c r="R5" t="s">
-        <v>9</v>
-      </c>
-      <c r="S5" t="s">
-        <v>5</v>
-      </c>
-      <c r="T5" t="s">
-        <v>5</v>
-      </c>
-      <c r="U5" t="s">
-        <v>8</v>
-      </c>
-      <c r="V5" t="s">
-        <v>4</v>
-      </c>
-      <c r="W5" t="s">
-        <v>12</v>
-      </c>
-      <c r="X5" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:24">
       <c r="A6">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
@@ -1153,84 +1153,84 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I6" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J6" t="s">
         <v>5</v>
       </c>
       <c r="K6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="N6" t="s">
         <v>5</v>
       </c>
       <c r="O6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="P6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Q6" t="s">
         <v>3</v>
       </c>
       <c r="R6" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="S6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="U6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="V6" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="W6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="X6" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:24">
       <c r="A7">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G7" t="s">
         <v>3</v>
@@ -1239,49 +1239,49 @@
         <v>5</v>
       </c>
       <c r="I7" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="L7" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="M7" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="N7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O7" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="P7" t="s">
         <v>3</v>
       </c>
       <c r="Q7" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="R7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="S7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="T7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="U7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V7" t="s">
         <v>11</v>
       </c>
       <c r="W7" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="X7" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
mes experimentations carts ok
</commit_message>
<xml_diff>
--- a/resultatsEvscape.xlsx
+++ b/resultatsEvscape.xlsx
@@ -23,106 +23,106 @@
     <t>Khalid</t>
   </si>
   <si>
+    <t>responseA</t>
+  </si>
+  <si>
+    <t>Reponse2Spec1</t>
+  </si>
+  <si>
+    <t>reponseC</t>
+  </si>
+  <si>
+    <t>abstention</t>
+  </si>
+  <si>
+    <t>reponseB</t>
+  </si>
+  <si>
     <t>Reponse1Spec1</t>
   </si>
   <si>
-    <t>reponseB</t>
-  </si>
-  <si>
-    <t>abstention</t>
-  </si>
-  <si>
-    <t>responseA</t>
-  </si>
-  <si>
     <t>Reponse7Spec1</t>
   </si>
   <si>
-    <t>reponseC</t>
-  </si>
-  <si>
-    <t>Reponse2Spec1</t>
+    <t>Reponse8Spec1</t>
+  </si>
+  <si>
+    <t>Reponse9Spec1</t>
+  </si>
+  <si>
+    <t>Tozer</t>
+  </si>
+  <si>
+    <t>Elie</t>
   </si>
   <si>
     <t>Reponse3Spec1</t>
   </si>
   <si>
+    <t>Reponse4Spec1</t>
+  </si>
+  <si>
+    <t>Reponse10Spec1</t>
+  </si>
+  <si>
+    <t>Patricke</t>
+  </si>
+  <si>
+    <t>Kluivert</t>
+  </si>
+  <si>
+    <t>Patrke</t>
+  </si>
+  <si>
+    <t>Klert</t>
+  </si>
+  <si>
+    <t>Berrd</t>
+  </si>
+  <si>
+    <t>Aert</t>
+  </si>
+  <si>
+    <t>Lita</t>
+  </si>
+  <si>
+    <t>Zoe</t>
+  </si>
+  <si>
     <t>Reponse6Spec1</t>
   </si>
   <si>
-    <t>Reponse8Spec1</t>
-  </si>
-  <si>
-    <t>Reponse9Spec1</t>
-  </si>
-  <si>
     <t>toto</t>
   </si>
   <si>
     <t>litoe</t>
   </si>
   <si>
-    <t>Reponse4Spec1</t>
-  </si>
-  <si>
-    <t>Reponse10Spec1</t>
-  </si>
-  <si>
     <t>Gisele</t>
   </si>
   <si>
     <t>Giligi</t>
   </si>
   <si>
-    <t>Patricke</t>
-  </si>
-  <si>
-    <t>Kluivert</t>
+    <t>Reponse5Spec1</t>
+  </si>
+  <si>
+    <t>Bernard</t>
+  </si>
+  <si>
+    <t>Albert</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>lie</t>
   </si>
   <si>
     <t>Gele</t>
   </si>
   <si>
     <t>Gigi</t>
-  </si>
-  <si>
-    <t>Reponse5Spec1</t>
-  </si>
-  <si>
-    <t>Berrd</t>
-  </si>
-  <si>
-    <t>Aert</t>
-  </si>
-  <si>
-    <t>Tozer</t>
-  </si>
-  <si>
-    <t>Elie</t>
-  </si>
-  <si>
-    <t>Lita</t>
-  </si>
-  <si>
-    <t>Zoe</t>
-  </si>
-  <si>
-    <t>Bernard</t>
-  </si>
-  <si>
-    <t>Albert</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>lie</t>
-  </si>
-  <si>
-    <t>Patrke</t>
-  </si>
-  <si>
-    <t>Klert</t>
   </si>
 </sst>
 </file>
@@ -454,158 +454,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A8:X12"/>
+  <dimension ref="A7:X12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
+    <row r="7" spans="1:24">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" t="s">
+        <v>5</v>
+      </c>
+      <c r="L7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" t="s">
+        <v>10</v>
+      </c>
+      <c r="N7" t="s">
+        <v>4</v>
+      </c>
+      <c r="O7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>5</v>
+      </c>
+      <c r="R7" t="s">
+        <v>14</v>
+      </c>
+      <c r="S7" t="s">
+        <v>2</v>
+      </c>
+      <c r="T7" t="s">
+        <v>24</v>
+      </c>
+      <c r="U7" t="s">
+        <v>8</v>
+      </c>
+      <c r="V7" t="s">
+        <v>9</v>
+      </c>
+      <c r="W7" t="s">
+        <v>4</v>
+      </c>
+      <c r="X7" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="8" spans="1:24">
       <c r="A8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
         <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J8" t="s">
+        <v>5</v>
+      </c>
+      <c r="K8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" t="s">
+        <v>9</v>
+      </c>
+      <c r="M8" t="s">
         <v>10</v>
       </c>
-      <c r="K8" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" t="s">
-        <v>3</v>
-      </c>
-      <c r="M8" t="s">
-        <v>4</v>
-      </c>
       <c r="N8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="P8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="Q8" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="S8" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="T8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U8" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="V8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="W8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="X8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:24">
       <c r="A9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" t="s">
         <v>28</v>
-      </c>
-      <c r="C9" t="s">
-        <v>29</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K9" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" t="s">
+        <v>4</v>
+      </c>
+      <c r="M9" t="s">
+        <v>4</v>
+      </c>
+      <c r="N9" t="s">
+        <v>5</v>
+      </c>
+      <c r="O9" t="s">
+        <v>5</v>
+      </c>
+      <c r="P9" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>13</v>
+      </c>
+      <c r="R9" t="s">
+        <v>14</v>
+      </c>
+      <c r="S9" t="s">
+        <v>29</v>
+      </c>
+      <c r="T9" t="s">
+        <v>2</v>
+      </c>
+      <c r="U9" t="s">
         <v>8</v>
       </c>
-      <c r="G9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" t="s">
-        <v>3</v>
-      </c>
-      <c r="I9" t="s">
-        <v>3</v>
-      </c>
-      <c r="J9" t="s">
-        <v>4</v>
-      </c>
-      <c r="K9" t="s">
-        <v>5</v>
-      </c>
-      <c r="L9" t="s">
-        <v>5</v>
-      </c>
-      <c r="M9" t="s">
-        <v>3</v>
-      </c>
-      <c r="N9" t="s">
-        <v>4</v>
-      </c>
-      <c r="O9" t="s">
-        <v>4</v>
-      </c>
-      <c r="P9" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>4</v>
-      </c>
-      <c r="R9" t="s">
+      <c r="V9" t="s">
+        <v>9</v>
+      </c>
+      <c r="W9" t="s">
+        <v>5</v>
+      </c>
+      <c r="X9" t="s">
         <v>15</v>
-      </c>
-      <c r="S9" t="s">
-        <v>4</v>
-      </c>
-      <c r="T9" t="s">
-        <v>3</v>
-      </c>
-      <c r="U9" t="s">
-        <v>6</v>
-      </c>
-      <c r="V9" t="s">
-        <v>7</v>
-      </c>
-      <c r="W9" t="s">
-        <v>12</v>
-      </c>
-      <c r="X9" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:24">
@@ -622,31 +696,31 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G10" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J10" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="K10" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L10" t="s">
         <v>5</v>
       </c>
       <c r="M10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N10" t="s">
         <v>5</v>
@@ -655,31 +729,31 @@
         <v>2</v>
       </c>
       <c r="P10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Q10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="R10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="S10" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="T10" t="s">
+        <v>5</v>
+      </c>
+      <c r="U10" t="s">
+        <v>5</v>
+      </c>
+      <c r="V10" t="s">
+        <v>2</v>
+      </c>
+      <c r="W10" t="s">
         <v>10</v>
       </c>
-      <c r="U10" t="s">
-        <v>6</v>
-      </c>
-      <c r="V10" t="s">
-        <v>11</v>
-      </c>
-      <c r="W10" t="s">
-        <v>4</v>
-      </c>
       <c r="X10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:24">
@@ -696,69 +770,69 @@
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I11" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="J11" t="s">
         <v>4</v>
       </c>
       <c r="K11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M11" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O11" t="s">
         <v>7</v>
       </c>
       <c r="P11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q11" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="R11" t="s">
         <v>5</v>
       </c>
       <c r="S11" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="T11" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="U11" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="V11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="W11" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="X11" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:24">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>34</v>
@@ -770,64 +844,64 @@
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G12" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H12" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="I12" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J12" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K12" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N12" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O12" t="s">
         <v>7</v>
       </c>
       <c r="P12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Q12" t="s">
+        <v>5</v>
+      </c>
+      <c r="R12" t="s">
+        <v>2</v>
+      </c>
+      <c r="S12" t="s">
+        <v>4</v>
+      </c>
+      <c r="T12" t="s">
+        <v>4</v>
+      </c>
+      <c r="U12" t="s">
+        <v>4</v>
+      </c>
+      <c r="V12" t="s">
         <v>9</v>
       </c>
-      <c r="R12" t="s">
-        <v>5</v>
-      </c>
-      <c r="S12" t="s">
-        <v>3</v>
-      </c>
-      <c r="T12" t="s">
-        <v>5</v>
-      </c>
-      <c r="U12" t="s">
-        <v>5</v>
-      </c>
-      <c r="V12" t="s">
-        <v>11</v>
-      </c>
       <c r="W12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="X12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -837,7 +911,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:X7"/>
+  <dimension ref="A2:X6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -863,69 +937,69 @@
         <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J2" t="s">
         <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" t="s">
         <v>7</v>
       </c>
-      <c r="N2" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" t="s">
-        <v>2</v>
-      </c>
       <c r="P2" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" t="s">
+        <v>5</v>
+      </c>
+      <c r="U2" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="V2" t="s">
         <v>9</v>
       </c>
-      <c r="R2" t="s">
-        <v>4</v>
-      </c>
-      <c r="S2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="W2" t="s">
         <v>10</v>
       </c>
-      <c r="U2" t="s">
-        <v>6</v>
-      </c>
-      <c r="V2" t="s">
-        <v>11</v>
-      </c>
-      <c r="W2" t="s">
-        <v>12</v>
-      </c>
       <c r="X2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:24">
       <c r="A3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -934,72 +1008,72 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H3" t="s">
         <v>5</v>
       </c>
       <c r="I3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N3" t="s">
         <v>4</v>
       </c>
       <c r="O3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="P3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Q3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="R3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" t="s">
+        <v>5</v>
+      </c>
+      <c r="U3" t="s">
+        <v>5</v>
+      </c>
+      <c r="V3" t="s">
+        <v>4</v>
+      </c>
+      <c r="W3" t="s">
+        <v>5</v>
+      </c>
+      <c r="X3" t="s">
         <v>15</v>
-      </c>
-      <c r="S3" t="s">
-        <v>7</v>
-      </c>
-      <c r="T3" t="s">
-        <v>10</v>
-      </c>
-      <c r="U3" t="s">
-        <v>5</v>
-      </c>
-      <c r="V3" t="s">
-        <v>4</v>
-      </c>
-      <c r="W3" t="s">
-        <v>12</v>
-      </c>
-      <c r="X3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:24">
       <c r="A4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -1011,69 +1085,69 @@
         <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="I4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="M4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="N4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="O4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P4" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>13</v>
+      </c>
+      <c r="R4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S4" t="s">
+        <v>6</v>
+      </c>
+      <c r="T4" t="s">
+        <v>4</v>
+      </c>
+      <c r="U4" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="V4" t="s">
         <v>9</v>
       </c>
-      <c r="R4" t="s">
-        <v>3</v>
-      </c>
-      <c r="S4" t="s">
-        <v>3</v>
-      </c>
-      <c r="T4" t="s">
-        <v>3</v>
-      </c>
-      <c r="U4" t="s">
-        <v>7</v>
-      </c>
-      <c r="V4" t="s">
-        <v>4</v>
-      </c>
       <c r="W4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="X4" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:24">
       <c r="A5">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
         <v>19</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -1082,10 +1156,10 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H5" t="s">
         <v>4</v>
@@ -1094,197 +1168,123 @@
         <v>4</v>
       </c>
       <c r="J5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="O5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R5" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="S5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="T5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="X5" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:24">
       <c r="A6">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
         <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" t="s">
+        <v>4</v>
+      </c>
+      <c r="L6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M6" t="s">
+        <v>2</v>
+      </c>
+      <c r="N6" t="s">
+        <v>5</v>
+      </c>
+      <c r="O6" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" t="s">
         <v>3</v>
       </c>
-      <c r="H6" t="s">
-        <v>4</v>
-      </c>
-      <c r="I6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="Q6" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" t="s">
+        <v>5</v>
+      </c>
+      <c r="S6" t="s">
+        <v>5</v>
+      </c>
+      <c r="T6" t="s">
+        <v>4</v>
+      </c>
+      <c r="U6" t="s">
+        <v>8</v>
+      </c>
+      <c r="V6" t="s">
+        <v>9</v>
+      </c>
+      <c r="W6" t="s">
         <v>10</v>
       </c>
-      <c r="K6" t="s">
-        <v>4</v>
-      </c>
-      <c r="L6" t="s">
-        <v>4</v>
-      </c>
-      <c r="M6" t="s">
-        <v>4</v>
-      </c>
-      <c r="N6" t="s">
-        <v>3</v>
-      </c>
-      <c r="O6" t="s">
-        <v>2</v>
-      </c>
-      <c r="P6" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>9</v>
-      </c>
-      <c r="R6" t="s">
-        <v>4</v>
-      </c>
-      <c r="S6" t="s">
-        <v>3</v>
-      </c>
-      <c r="T6" t="s">
-        <v>4</v>
-      </c>
-      <c r="U6" t="s">
-        <v>6</v>
-      </c>
-      <c r="V6" t="s">
-        <v>11</v>
-      </c>
-      <c r="W6" t="s">
-        <v>4</v>
-      </c>
       <c r="X6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24">
-      <c r="A7">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" t="s">
-        <v>3</v>
-      </c>
-      <c r="H7" t="s">
-        <v>3</v>
-      </c>
-      <c r="I7" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" t="s">
-        <v>4</v>
-      </c>
-      <c r="K7" t="s">
-        <v>4</v>
-      </c>
-      <c r="L7" t="s">
-        <v>4</v>
-      </c>
-      <c r="M7" t="s">
-        <v>4</v>
-      </c>
-      <c r="N7" t="s">
-        <v>4</v>
-      </c>
-      <c r="O7" t="s">
-        <v>2</v>
-      </c>
-      <c r="P7" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>9</v>
-      </c>
-      <c r="R7" t="s">
-        <v>7</v>
-      </c>
-      <c r="S7" t="s">
-        <v>5</v>
-      </c>
-      <c r="T7" t="s">
-        <v>5</v>
-      </c>
-      <c r="U7" t="s">
-        <v>4</v>
-      </c>
-      <c r="V7" t="s">
-        <v>11</v>
-      </c>
-      <c r="W7" t="s">
-        <v>12</v>
-      </c>
-      <c r="X7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
a priori tt fctionne
</commit_message>
<xml_diff>
--- a/resultatsEvscape.xlsx
+++ b/resultatsEvscape.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="36">
   <si>
     <t>Boudlal</t>
   </si>
@@ -26,22 +26,79 @@
     <t>responseA</t>
   </si>
   <si>
+    <t>abstention</t>
+  </si>
+  <si>
     <t>reponseB</t>
   </si>
   <si>
-    <t>abstention</t>
+    <t>Reponse7Spec1</t>
   </si>
   <si>
     <t>Reponse8Spec1</t>
   </si>
   <si>
+    <t>reponseC</t>
+  </si>
+  <si>
+    <t>Reponse10Spec1</t>
+  </si>
+  <si>
+    <t>Lita</t>
+  </si>
+  <si>
+    <t>Zoe</t>
+  </si>
+  <si>
+    <t>Reponse2Spec1</t>
+  </si>
+  <si>
+    <t>Reponse3Spec1</t>
+  </si>
+  <si>
     <t>Reponse9Spec1</t>
   </si>
   <si>
-    <t>reponseC</t>
-  </si>
-  <si>
-    <t>Reponse7Spec1</t>
+    <t>Patricke</t>
+  </si>
+  <si>
+    <t>Kluivert</t>
+  </si>
+  <si>
+    <t>Bernard</t>
+  </si>
+  <si>
+    <t>Albert</t>
+  </si>
+  <si>
+    <t>Reponse4Spec1</t>
+  </si>
+  <si>
+    <t>Reponse5Spec1</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>lie</t>
+  </si>
+  <si>
+    <t>Gele</t>
+  </si>
+  <si>
+    <t>Gigi</t>
+  </si>
+  <si>
+    <t>Reponse6Spec1</t>
+  </si>
+  <si>
+    <t>Berrd</t>
+  </si>
+  <si>
+    <t>Aert</t>
+  </si>
+  <si>
+    <t>Reponse1Spec1</t>
   </si>
   <si>
     <t>Tozer</t>
@@ -50,76 +107,22 @@
     <t>Elie</t>
   </si>
   <si>
-    <t>Reponse2Spec1</t>
-  </si>
-  <si>
-    <t>Lita</t>
-  </si>
-  <si>
-    <t>Zoe</t>
-  </si>
-  <si>
-    <t>Reponse1Spec1</t>
-  </si>
-  <si>
     <t>toto</t>
   </si>
   <si>
     <t>litoe</t>
   </si>
   <si>
-    <t>Reponse4Spec1</t>
-  </si>
-  <si>
-    <t>Reponse3Spec1</t>
-  </si>
-  <si>
     <t>Gisele</t>
   </si>
   <si>
     <t>Giligi</t>
   </si>
   <si>
-    <t>Reponse10Spec1</t>
-  </si>
-  <si>
-    <t>Patricke</t>
-  </si>
-  <si>
-    <t>Kluivert</t>
-  </si>
-  <si>
-    <t>Bernard</t>
-  </si>
-  <si>
-    <t>Albert</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>lie</t>
-  </si>
-  <si>
-    <t>Gele</t>
-  </si>
-  <si>
-    <t>Gigi</t>
-  </si>
-  <si>
     <t>Patrke</t>
   </si>
   <si>
     <t>Klert</t>
-  </si>
-  <si>
-    <t>Reponse5Spec1</t>
-  </si>
-  <si>
-    <t>Berrd</t>
-  </si>
-  <si>
-    <t>Aert</t>
   </si>
 </sst>
 </file>
@@ -459,64 +462,64 @@
   <sheetData>
     <row r="9" spans="1:24">
       <c r="A9">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="F9" t="s">
         <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="I9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K9" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="M9" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O9" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="P9" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="Q9" t="s">
         <v>4</v>
       </c>
       <c r="R9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="T9" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="U9" t="s">
         <v>4</v>
@@ -525,232 +528,232 @@
         <v>7</v>
       </c>
       <c r="W9" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="X9" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:24">
       <c r="A10">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D10" t="b">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G10" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="J10" t="s">
         <v>3</v>
       </c>
       <c r="K10" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L10" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O10" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="P10" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="Q10" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="R10" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="S10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T10" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U10" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="V10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="W10" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="X10" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:24">
       <c r="A11">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H11" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I11" t="s">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="J11" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M11" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="N11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O11" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="P11" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q11" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="R11" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="S11" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="T11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U11" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V11" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="X11" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:24">
       <c r="A12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
       </c>
       <c r="G12" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H12" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L12" t="s">
         <v>3</v>
       </c>
       <c r="M12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N12" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O12" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="P12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Q12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R12" t="s">
         <v>3</v>
       </c>
       <c r="S12" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="T12" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="U12" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="V12" t="s">
         <v>4</v>
       </c>
       <c r="W12" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="X12" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -792,57 +795,57 @@
         <v>4</v>
       </c>
       <c r="I2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K2" t="s">
         <v>3</v>
       </c>
       <c r="L2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M2" t="s">
+        <v>4</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R2" t="s">
+        <v>3</v>
+      </c>
+      <c r="S2" t="s">
+        <v>2</v>
+      </c>
+      <c r="T2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" t="s">
         <v>5</v>
       </c>
-      <c r="M2" t="s">
+      <c r="V2" t="s">
         <v>6</v>
       </c>
-      <c r="N2" t="s">
-        <v>4</v>
-      </c>
-      <c r="O2" t="s">
-        <v>4</v>
-      </c>
-      <c r="P2" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>4</v>
-      </c>
-      <c r="R2" t="s">
-        <v>4</v>
-      </c>
-      <c r="S2" t="s">
-        <v>4</v>
-      </c>
-      <c r="T2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
+        <v>7</v>
+      </c>
+      <c r="X2" t="s">
         <v>8</v>
-      </c>
-      <c r="V2" t="s">
-        <v>5</v>
-      </c>
-      <c r="W2" t="s">
-        <v>6</v>
-      </c>
-      <c r="X2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:24">
       <c r="A3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -854,61 +857,61 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I3" t="s">
         <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L3" t="s">
         <v>7</v>
       </c>
       <c r="M3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="O3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="P3" t="s">
         <v>11</v>
       </c>
       <c r="Q3" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="R3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="S3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="U3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="V3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="W3" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="X3" t="s">
         <v>3</v>
@@ -916,58 +919,58 @@
     </row>
     <row r="4" spans="1:24">
       <c r="A4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G4" t="s">
         <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="L4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="N4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="O4" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="P4" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="Q4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="S4" t="s">
         <v>3</v>
@@ -976,27 +979,27 @@
         <v>4</v>
       </c>
       <c r="U4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="V4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="W4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="X4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:24">
       <c r="A5">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -1005,58 +1008,58 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I5" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="J5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="N5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O5" t="s">
         <v>3</v>
       </c>
       <c r="P5" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="Q5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="R5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S5" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="T5" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="U5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="V5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W5" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="X5" t="s">
         <v>3</v>
@@ -1064,81 +1067,81 @@
     </row>
     <row r="6" spans="1:24">
       <c r="A6">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F6" t="s">
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J6" t="s">
         <v>3</v>
       </c>
       <c r="K6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M6" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="N6" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="O6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P6" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="Q6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T6" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="U6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="V6" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="W6" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="X6" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:24">
       <c r="A7">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
@@ -1150,75 +1153,75 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H7" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="I7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J7" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="K7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L7" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M7" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="N7" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="O7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P7" t="s">
         <v>11</v>
       </c>
       <c r="Q7" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="R7" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="S7" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="T7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U7" t="s">
+        <v>5</v>
+      </c>
+      <c r="V7" t="s">
+        <v>3</v>
+      </c>
+      <c r="W7" t="s">
+        <v>2</v>
+      </c>
+      <c r="X7" t="s">
         <v>8</v>
-      </c>
-      <c r="V7" t="s">
-        <v>7</v>
-      </c>
-      <c r="W7" t="s">
-        <v>2</v>
-      </c>
-      <c r="X7" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:24">
       <c r="A8">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" t="b">
         <v>1</v>
@@ -1227,25 +1230,25 @@
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L8" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M8" t="s">
         <v>2</v>
@@ -1254,34 +1257,34 @@
         <v>7</v>
       </c>
       <c r="O8" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="P8" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="Q8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="R8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S8" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="T8" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="U8" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="V8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W8" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="X8" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>